<commit_message>
end report changes and small implementation changes
</commit_message>
<xml_diff>
--- a/scrumrelaterat/sprint_backlog.xlsx
+++ b/scrumrelaterat/sprint_backlog.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="15105" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="210" windowWidth="15105" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
   <si>
     <t>week</t>
   </si>
@@ -81,9 +81,6 @@
     <t>TODO/canceled</t>
   </si>
   <si>
-    <t>Start building the analyzer in Matlab.</t>
-  </si>
-  <si>
     <t>research gui components in the plugin tool</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>40-41</t>
   </si>
   <si>
-    <t>Paul &amp; (Razmus)</t>
-  </si>
-  <si>
     <t>Extract more trace data with relevant propsim settings</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>build basic analyzing script in Java</t>
   </si>
   <si>
-    <t>Start building the analyzer-plugin to logtool in Java.</t>
-  </si>
-  <si>
     <t>Find more relevant articles about HARQ and LA</t>
   </si>
   <si>
@@ -139,6 +130,42 @@
   </si>
   <si>
     <t>Plan interview</t>
+  </si>
+  <si>
+    <t>42-43</t>
+  </si>
+  <si>
+    <t>44-45</t>
+  </si>
+  <si>
+    <t>plan analysation of Link Adaptation</t>
+  </si>
+  <si>
+    <t>build the analyzer-plugin to logtool in Java.</t>
+  </si>
+  <si>
+    <t>Plan analysation of HARQ</t>
+  </si>
+  <si>
+    <t>TODO?</t>
+  </si>
+  <si>
+    <t>46-47</t>
+  </si>
+  <si>
+    <t>Save graphs</t>
+  </si>
+  <si>
+    <t>licensavtal för jfreechart, vad gäller. Höra med logtool</t>
+  </si>
+  <si>
+    <t>fix the optional tab in the analyser</t>
+  </si>
+  <si>
+    <t>Can we save energy if we reduce the number of harq process, or something similar</t>
+  </si>
+  <si>
+    <t>create an realtime analyser in the plugin</t>
   </si>
 </sst>
 </file>
@@ -509,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H27"/>
+  <dimension ref="B3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +547,9 @@
     <col min="3" max="3" width="66.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="72.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -548,7 +577,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -557,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="6">
         <v>41901</v>
@@ -574,7 +603,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -585,7 +614,7 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="6">
         <v>41900</v>
@@ -602,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6">
         <v>41904</v>
@@ -616,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="6">
         <v>41904</v>
@@ -624,13 +653,13 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -641,7 +670,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -652,7 +681,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="6">
         <v>41902</v>
@@ -666,21 +695,21 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="6">
         <v>41913</v>
@@ -691,19 +720,19 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="6">
         <v>41929</v>
       </c>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -714,29 +743,29 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="6">
         <v>41902</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F17" s="6">
-        <v>41913</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+        <v>41911</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>10</v>
@@ -745,105 +774,106 @@
         <v>24</v>
       </c>
       <c r="F18" s="6">
-        <v>41911</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+        <v>41908</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="6">
-        <v>41908</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F20" s="6">
+        <v>41914</v>
+      </c>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="6">
+        <v>41913</v>
+      </c>
+      <c r="G23" s="6">
+        <v>41915</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="6">
-        <v>41914</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="F24" s="6">
+        <v>41920</v>
+      </c>
+      <c r="G24" s="6">
+        <v>41920</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="6">
-        <v>41913</v>
-      </c>
-      <c r="G24" s="6">
-        <v>41915</v>
-      </c>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F25" s="6">
-        <v>41920</v>
-      </c>
-      <c r="G25" s="6">
-        <v>41920</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+        <v>41921</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>37</v>
       </c>
@@ -851,21 +881,342 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="6">
-        <v>41921</v>
-      </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="6">
+        <v>41902</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="6">
+        <v>41911</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="6">
+        <v>41918</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6">
+        <v>41936</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="6">
+        <v>41902</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="6">
+        <v>41911</v>
+      </c>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="6">
+        <v>41939</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="6">
+        <v>41939</v>
+      </c>
+      <c r="G41" s="6">
+        <v>41942</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="6">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G47" s="6"/>
+      <c r="H47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E27" t="s">
-        <v>25</v>
+      <c r="E48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="6">
+        <v>41902</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s">
+        <v>23</v>
+      </c>
+      <c r="F50" s="6">
+        <v>41911</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="6">
+        <v>41939</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" s="6">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="6">
+        <v>41953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
andrat i basicview funktioner
</commit_message>
<xml_diff>
--- a/scrumrelaterat/sprint_backlog.xlsx
+++ b/scrumrelaterat/sprint_backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="81">
   <si>
     <t>week</t>
   </si>
@@ -219,31 +219,46 @@
     <t>find a scientific base (articles) that the new analysation can be based on</t>
   </si>
   <si>
-    <t>prel 02-dec</t>
-  </si>
-  <si>
     <t>50-51</t>
   </si>
   <si>
-    <t>write questions to planneringsrapport</t>
-  </si>
-  <si>
-    <t>create opimization function in the tool</t>
-  </si>
-  <si>
-    <t>writing on the end report</t>
-  </si>
-  <si>
-    <t>create an enkät for testers.</t>
-  </si>
-  <si>
-    <t>the testers answer the enkät on how well designed the tool is.</t>
-  </si>
-  <si>
-    <t>make testers test our tool</t>
-  </si>
-  <si>
-    <t>draw traces for the analysis on BLER target</t>
+    <t>The articles is now about BLER vs Throughput</t>
+  </si>
+  <si>
+    <t>Have a demo for the tester at IODT</t>
+  </si>
+  <si>
+    <t>add automatic analysation for the tool</t>
+  </si>
+  <si>
+    <t>The Demo is between 14-15 at Monday</t>
+  </si>
+  <si>
+    <t>Create a servey for the testers</t>
+  </si>
+  <si>
+    <t>The servey will be question on how good the tool is, easy to use etc...</t>
+  </si>
+  <si>
+    <t>Draw traces with different BLER settings.</t>
+  </si>
+  <si>
+    <t>Do analysation on the trace data + test the automatic analyse tool</t>
+  </si>
+  <si>
+    <t>Bug fixing + redesign of the tool</t>
+  </si>
+  <si>
+    <t>Fix bugs, optimize code, change view layout etc.</t>
+  </si>
+  <si>
+    <t>(Paul) &amp; Razmus</t>
+  </si>
+  <si>
+    <t>look at which the optimal bler target is + calculate it with the automation function</t>
+  </si>
+  <si>
+    <t>prel 5-dec</t>
   </si>
 </sst>
 </file>
@@ -621,17 +636,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H74"/>
+  <dimension ref="B3:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="69" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="72.140625" customWidth="1"/>
@@ -1362,14 +1377,20 @@
       <c r="C60" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>53</v>
+      <c r="D60" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E60" t="s">
         <v>24</v>
       </c>
       <c r="F60" s="6">
         <v>41939</v>
+      </c>
+      <c r="G60" s="6">
+        <v>41975</v>
+      </c>
+      <c r="H60" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -1430,8 +1451,8 @@
       <c r="C64" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>9</v>
+      <c r="D64" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E64" t="s">
         <v>24</v>
@@ -1439,8 +1460,8 @@
       <c r="F64" s="6">
         <v>41969</v>
       </c>
-      <c r="G64" s="6" t="s">
-        <v>67</v>
+      <c r="G64" s="6">
+        <v>41975</v>
       </c>
       <c r="H64" t="s">
         <v>62</v>
@@ -1450,22 +1471,25 @@
       <c r="C65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>9</v>
+      <c r="D65" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E65" t="s">
         <v>64</v>
       </c>
       <c r="F65" s="6">
         <v>41970</v>
+      </c>
+      <c r="G65" s="6">
+        <v>41975</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>9</v>
+      <c r="D66" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E66" t="s">
         <v>23</v>
@@ -1473,16 +1497,16 @@
       <c r="F66" s="6">
         <v>41970</v>
       </c>
-      <c r="G66" s="6" t="s">
-        <v>67</v>
+      <c r="G66" s="6">
+        <v>41977</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>9</v>
+      <c r="D67" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E67" t="s">
         <v>22</v>
@@ -1490,42 +1514,149 @@
       <c r="F67" s="6">
         <v>41970</v>
       </c>
-      <c r="G67" s="6"/>
+      <c r="G67" s="6">
+        <v>41975</v>
+      </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C69" t="s">
+        <v>48</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E69" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" s="6"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
-        <v>75</v>
+        <v>11</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E70" t="s">
+        <v>24</v>
+      </c>
+      <c r="F70" s="6">
+        <v>41902</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
-        <v>70</v>
+        <v>41</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E71" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71" s="6">
+        <v>41911</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
-        <v>71</v>
+        <v>47</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E72" t="s">
+        <v>23</v>
+      </c>
+      <c r="F72" s="6">
+        <v>41953</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="6">
+        <v>41981</v>
       </c>
       <c r="H73" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C74" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>23</v>
+      </c>
+      <c r="H75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>22</v>
+      </c>
+      <c r="F76" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C77" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>22</v>
+      </c>
+      <c r="H77" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C78" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" t="s">
+        <v>78</v>
+      </c>
+      <c r="F78" s="6">
+        <v>41973</v>
+      </c>
+      <c r="H78" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>